<commit_message>
even more changes to algo assign
</commit_message>
<xml_diff>
--- a/Algorithmics/Sheet1.xlsx
+++ b/Algorithmics/Sheet1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Semester2\Algorithmics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\Study\Algorithmics\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08732B57-0222-4BD2-8498-1C6C8693486C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7896"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -37,11 +38,20 @@
   <si>
     <t>Quick sort</t>
   </si>
+  <si>
+    <t>28 for 250000</t>
+  </si>
+  <si>
+    <t>x for 10000000000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -72,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -103,7 +114,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -120,7 +131,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -153,18 +164,17 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>LOG</a:t>
+              <a:rPr lang="en-GB"/>
+              <a:t>LOG-LOG</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> LOG AVERAGE RUN TIME</a:t>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> INSERTION SORT</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -190,7 +200,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="bg-BG"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -198,14 +208,14 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -240,10 +250,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:formatCode>0.00;[Red]0.00</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -264,16 +274,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>Sheet1!$B$12:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>6.03624E-3</c:v>
                 </c:pt>
@@ -281,7 +294,7 @@
                   <c:v>2.644268E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.3343700000000003E-2</c:v>
+                  <c:v>5.9998999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.5515098599999999</c:v>
@@ -294,18 +307,26 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>441.5884757</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EC47-443D-AC5E-7FC4572C599E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -340,10 +361,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:formatCode>0.00;[Red]0.00</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -364,16 +385,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:f>Sheet1!$B$13:$I$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>6.8517999999999997E-4</c:v>
                 </c:pt>
@@ -398,14 +422,19 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EC47-443D-AC5E-7FC4572C599E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -440,10 +469,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:formatCode>0.00;[Red]0.00</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -464,21 +493,24 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>Sheet1!$B$14:$I$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>8.1492000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1170199999999999E-3</c:v>
+                  <c:v>5.0989199999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.0989199999999998E-3</c:v>
@@ -498,7 +530,12 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EC47-443D-AC5E-7FC4572C599E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -508,11 +545,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="482776896"/>
-        <c:axId val="482778856"/>
+        <c:axId val="62121263"/>
+        <c:axId val="59313279"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="482776896"/>
+        <c:axId val="62121263"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -534,81 +571,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:minorGridlines>
+        <c:numFmt formatCode="0.00;[Red]0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="59313279"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="59313279"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>LOG SIZE</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> OF INPUT</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="bg-BG"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -643,21 +668,253 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="bg-BG"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482778856"/>
+        <c:crossAx val="62121263"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$24:$E$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$24:$F$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F948-451D-9CEE-FB5B9E204509}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="69604623"/>
+        <c:axId val="2086854207"/>
+      </c:scatterChart>
       <c:valAx>
-        <c:axId val="482778856"/>
+        <c:axId val="69604623"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -672,76 +929,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>LOG AVERAGE RUN TIME</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="bg-BG"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -776,10 +963,73 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="bg-BG"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482776896"/>
+        <c:crossAx val="2086854207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2086854207"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69604623"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -791,40 +1041,15 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="bg-BG"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -849,7 +1074,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="bg-BG"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -900,6 +1125,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1416,24 +1681,546 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>195261</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E445C76-56E7-40E1-A411-F555327B3DB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1443,6 +2230,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>176212</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FC33334-CCD6-4E49-9E97-3DD8733226BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1713,16 +2536,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1736,7 +2566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -1750,7 +2580,7 @@
         <v>8.1492000000000001E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5000</v>
       </c>
@@ -1764,7 +2594,7 @@
         <v>3.1170199999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10000</v>
       </c>
@@ -1778,7 +2608,7 @@
         <v>5.0989199999999998E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50000</v>
       </c>
@@ -1792,7 +2622,7 @@
         <v>1.261724E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>100000</v>
       </c>
@@ -1806,7 +2636,7 @@
         <v>2.226566E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>250000</v>
       </c>
@@ -1820,7 +2650,7 @@
         <v>9.4847600000000004E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000000</v>
       </c>
@@ -1832,10 +2662,176 @@
       </c>
       <c r="D8">
         <v>0.20149829999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D11" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E11" s="1">
+        <v>50000</v>
+      </c>
+      <c r="F11" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G11" s="1">
+        <v>250000</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="I11" s="1">
+        <v>10000000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>6.03624E-3</v>
+      </c>
+      <c r="C12">
+        <v>2.644268E-2</v>
+      </c>
+      <c r="D12">
+        <v>5.9998999999999997E-2</v>
+      </c>
+      <c r="E12">
+        <v>1.5515098599999999</v>
+      </c>
+      <c r="F12">
+        <v>4.7312250999999996</v>
+      </c>
+      <c r="G12">
+        <v>27.940746900000001</v>
+      </c>
+      <c r="H12">
+        <v>441.5884757</v>
+      </c>
+      <c r="I12">
+        <v>10000000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>6.8517999999999997E-4</v>
+      </c>
+      <c r="C13">
+        <v>2.2712600000000002E-3</v>
+      </c>
+      <c r="D13">
+        <v>4.0097199999999996E-3</v>
+      </c>
+      <c r="E13">
+        <v>8.9246599999999992E-3</v>
+      </c>
+      <c r="F13">
+        <v>1.7207879999999998E-2</v>
+      </c>
+      <c r="G13">
+        <v>4.5159600000000001E-2</v>
+      </c>
+      <c r="H13">
+        <v>0.2275143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>8.1492000000000001E-4</v>
+      </c>
+      <c r="C14">
+        <v>5.0989199999999998E-3</v>
+      </c>
+      <c r="D14">
+        <v>5.0989199999999998E-3</v>
+      </c>
+      <c r="E14">
+        <v>1.261724E-2</v>
+      </c>
+      <c r="F14">
+        <v>2.226566E-2</v>
+      </c>
+      <c r="G14">
+        <v>9.4847600000000004E-2</v>
+      </c>
+      <c r="H14">
+        <v>0.20149829999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>100</v>
+      </c>
+      <c r="F26">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>1000</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>8000</v>
+      </c>
+      <c r="F28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>20000</v>
+      </c>
+      <c r="F29">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding a little more to algorithms
</commit_message>
<xml_diff>
--- a/Algorithmics/Sheet1.xlsx
+++ b/Algorithmics/Sheet1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\Study\Algorithmics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08732B57-0222-4BD2-8498-1C6C8693486C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462325E1-0B99-45B2-A84A-85805C0DF1EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1085,6 +1085,757 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insertion Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00;[Red]0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.03624E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.644268E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9998999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5515098599999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7312250999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.940746900000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>441.5884757</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9CC6-4991-9DFD-64FE291C71AE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1672320079"/>
+        <c:axId val="1598317391"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1672320079"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00;[Red]0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1598317391"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1598317391"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1672320079"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.03624E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.644268E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3343700000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5515098599999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7312250999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.940746900000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>441.5884757</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-062B-40E4-BA8A-9450089551BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1848433839"/>
+        <c:axId val="1593212575"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1848433839"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1593212575"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1593212575"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1848433839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1165,6 +1916,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2197,20 +3028,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>195261</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>185736</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2237,16 +4100,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>71437</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>176212</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>195262</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2266,6 +4129,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>366711</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5C1728E-5DC8-4652-A62C-461589F5F589}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>33337</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{697A2B42-CFDB-46C0-9C81-F867BA0701E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2539,8 +4474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>